<commit_message>
change database schema for target
</commit_message>
<xml_diff>
--- a/etl_test/dev_target.xlsx
+++ b/etl_test/dev_target.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurence/workspace/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6EEC83DB-7B7F-8142-96D5-1B9F6D803D9F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{692ACE2C-7F6B-6141-AD4B-BA7D3FFDC68C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5460" yWindow="2300" windowWidth="27860" windowHeight="17060" xr2:uid="{23907217-0933-3B43-83A8-2AA2AC99F6DE}"/>
+    <workbookView xWindow="9040" yWindow="2920" windowWidth="27860" windowHeight="17060" xr2:uid="{23907217-0933-3B43-83A8-2AA2AC99F6DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
@@ -25,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Start Date</t>
-  </si>
-  <si>
-    <t>End Date</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>Sales</t>
   </si>
@@ -43,15 +37,23 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>sales name A2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>sales name A3</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>lead name A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>time period</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019 Q2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sales name A2</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -428,82 +430,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F4AC9D7-A8FC-9B41-98B5-2B12A08EA77A}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="16">
+    <row r="1" spans="1:3" ht="16">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="16">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C2" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="16">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C4" s="2">
+        <v>300</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="16">
-      <c r="A2" s="1">
-        <v>201904</v>
-      </c>
-      <c r="B2" s="1">
-        <v>201906</v>
-      </c>
-      <c r="C2" s="1" t="s">
+    <row r="5" spans="1:3" ht="16">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2">
-        <v>20000000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16">
-      <c r="A3" s="1">
-        <v>201904</v>
-      </c>
-      <c r="B3" s="1">
-        <v>201906</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2">
-        <v>20000000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="16">
-      <c r="A4" s="1">
-        <v>201904</v>
-      </c>
-      <c r="B4" s="1">
-        <v>201906</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2">
-        <v>20000000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="16">
-      <c r="A5" s="1">
-        <v>201904</v>
-      </c>
-      <c r="B5" s="1">
-        <v>201906</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="2">
-        <v>20000000</v>
+      <c r="C5" s="2">
+        <v>400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>